<commit_message>
compare our translations with google and api
</commit_message>
<xml_diff>
--- a/reports/test_dataset_result.xlsx
+++ b/reports/test_dataset_result.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="284">
   <si>
     <t>Русский</t>
   </si>
@@ -725,6 +725,383 @@
     <t xml:space="preserve"> Новые протесты касаются представителей низшего среднего класса и бедных слоев населения и в основном относятся к провинциям и периферийным районам страны, в то время как " зеленое " движение, например, базировалось между высшим средним классом в крупных городах.
  В то время как в течение последних двух десятилетий протестующие в определенной степени симпатизировали так называемой &lt; &lt; исправительной фракции &gt; &gt; , новая волна протестов не только проводит различие между различными группировками режима, но и направлена против всего государства Исламская Республика -- института, который не только является репрессивным и жестоким, но и крайне коррумпированным и неэффективным.
 </t>
+  </si>
+  <si>
+    <t>google_ar-ru</t>
+  </si>
+  <si>
+    <t>api_ar-ru</t>
+  </si>
+  <si>
+    <t>Это дело было рассмотрено на основе тех же доказательств, которые были найдены не менее 10 лет назад. Если правосудие - это форма сдерживания людей от совершения преступлений, то безнаказанность в Колумбии является стимулом для совершения преступления, если осудить кого-то сложно, даже если они виноваты.</t>
+  </si>
+  <si>
+    <t>Государство должно публично осуждать насилие в отношении журналистов, проводить расследования и достоверно преследовать осужденных, а также сдерживать тех, кто сговаривается с целью совершения того же преступления в будущем.</t>
+  </si>
+  <si>
+    <t>Колумбийское [правительство] приняло программу защиты журналистов, находящихся под угрозой, которая все еще действует, но имеет противоречивую репутацию, особенно после того, как журналисты потеряли к ней доверие после подтверждения сговора между силами безопасности, ответственными за реализацию программы, и мишени для журналистов.</t>
+  </si>
+  <si>
+    <t>В сентябре Народная партия представила в парламент законопроект, в котором будет разработан Принцип индивидуального банкротства, который изменит правила привлечения к взысканию долгов. Хотя закон все еще находится на рассмотрении, его сторонники утверждают, что с таким уровнем защиты люди не будут лишены своего жилья. После выстрела со смертельным исходом в Алматы, крупнейшем городе страны, официальные лица назвали "жестокие" методы взыскания долгов главным мотивом стрелка.</t>
+  </si>
+  <si>
+    <t>Я также узнал много нового о художественном переводе. И я верю, что все еще учусь. Коммерческая сторона была очень ухабистой с точки зрения получения авторских прав и т. Д. Я начал книжный проект в 2017 году, и книга была наконец опубликована в 2020 году. Итак, помимо профессиональных и коммерческих аспектов, я научился искусству терпения и самодисциплины, чтобы продолжать, несмотря на препятствия.</t>
+  </si>
+  <si>
+    <t>И наконец, я хочу быть и делать то, что хочу видеть в мире. Если я хочу, чтобы принимали и читали более разнообразные книги из Южной Азии, я должен внести свой вклад в литературное гражданство. Я считаю, что вкладывать позитивную энергию в эту работу более продуктивно, чем просто жаловаться на те проблемы, которые я нахожу в литературной сфере. В настоящее время это индивидуальный риск, поскольку я не могу позволить себе заплатить одному из них, но я надеюсь найти некоторые варианты финансирования, чтобы я мог заплатить некоторым персонажам за обзоры и интервью. видеть.</t>
+  </si>
+  <si>
+    <t>История касается не здоровья заключенных, а здоровья самой страны. История заключается в репрессивных инструментах, унаследованных от поколений назад, и рассвет вражды будет унаследован для будущих поколений. Полное отрицание голоса и тела - суть зари в споре. Мы представляем себе, что это слово означает явное решение пойти дальше с враждебностью и причинением вреда. Но если вы меня видите и слышите, есть еще возможность отступить и успокоиться. И если мы не извлечем из этого пользу, мы, по крайней мере, продолжим пребывать в состоянии росы. Наивысший антагонизм в том, что вы меня не видите и не пытаетесь понять меня; Превратиться в субстанцию ​​только для того, чтобы вытеснить, истребить, затемнить, изгнать или исключить, превратиться в символ или пугало без физического тела. Рассвет в судебном процессе - это наследство, которое платят все органы, и вы продолжаете платить за него даже после завершения судебного процесса.</t>
+  </si>
+  <si>
+    <t>Как нам защитить тела наших детей от тюремного наследия? Ответ не заканчивается освобождением заключенных, но должен начинаться с освобождения и достигать воображения, которое стирает сами тюрьмы, а не заключенных.</t>
+  </si>
+  <si>
+    <t>Хотя Российская водородная стратегия является последним публичным документом и наиболее подробно описывает видение Кремля в отношении водорода, она далеко не кардинально меняет правила игры в энергетическом секторе страны. Фактически, как и многие другие подобные документы, которые должны стимулировать развитие российской энергетики, он, похоже, носит скорее реактивный, чем упреждающий характер, поскольку был принят более чем через год после того, как основные энергетические партнеры страны сформулировали свои водородные стратегии.</t>
+  </si>
+  <si>
+    <t>Некоторые называют водород швейцарским топливным ножом, и он во многих отношениях уникален. Поскольку это самый распространенный элемент во Вселенной, недостатка в его запасе не будет. Он может преобразовывать формы энергии из одной формы (электрической) в другую (химическую), хранить ее в течение длительного времени и транспортировать в нужное место. Однако примечательно то, что при горении он не выделяет углекислый газ. Фактически, в качестве побочного продукта образуется только вода.</t>
+  </si>
+  <si>
+    <t>Многие молодые сирийцы начали покидать юг Сирии с начала 2021 года из-за нестабильности в этом регионе и из-за опасений, что их отправят на обязательную службу в армию сирийского режима и бросят на фронты боевых действий на севере Сирии. страна. Многие из них продавали свои ценности в Сирии, чтобы получить деньги, чтобы заплатить контрабандистам в Ливии, чтобы доставить их на лодке в Италию и на Мальту через Средиземное море.</t>
+  </si>
+  <si>
+    <t>Мы собирались подойти к итальянскому побережью, а затем к лодке, на которую мы садились, подошел корабль, и они начали указывать на нас руками, мы решили убежать, но корабль спустил небольшую лодку с шестью вооруженными людьми, и они погнались за ней. после нас, а потом стреляли в двигатель нашей лодки, пока не смогли вывести его из строя, затем подошел корабль И нас перевели к нему, где было около 600 других иммигрантов разных национальностей.</t>
+  </si>
+  <si>
+    <t>ЕС несет ответственность за варварство Ливии напрямую или закрывая глаза на ее действия, поскольку вооруженные группы, получающие прибыль от мигрантов, финансируются, а соучастие в этих преступлениях остается безнаказанным из-за невозможности требовать ответственности и подотчетности в динамике переселения или аутсорсинге. миграционный контроль.</t>
+  </si>
+  <si>
+    <t>Помимо июньских выборов в Перу, как в Интернете, так и на самом деле распространялась дезинформация, касающаяся избирательного процесса, большая часть которой - как это наблюдается в других странах - была связана с попыткой подорвать доверие к избирательным органам, а также с мошенническим использованием ложных сведений. и реальная информация в политических целях; Например, распространение новостей о регистрации списков избирателей и указание на то, что списки включали имена умерших, но опускали информацию о расписании и процедуре внесения поправок и окончательной доработки списков.</t>
+  </si>
+  <si>
+    <t>Дезинформация распространилась во время этих протестов и демонстраций, вспыхнувших в Колумбии, поскольку местные источники сообщили, что в сети были распространены сотни видео, аудиозаписей и фотографий о забастовке в Колумбии по всей стране, и содержание содержало много лжи, что сильно повлияло на что творилось На улицах происходили реальные события.</t>
+  </si>
+  <si>
+    <t>Насилие также происходило вне рамок народных демонстраций, и участились разговоры о словесных и физических нападках на прессу со стороны государственных чиновников, занимающих высокие посты, и с января 2021 года в Латинской Америке были убиты по меньшей мере четыре журналиста.</t>
+  </si>
+  <si>
+    <t>Теперь, когда Талибан находится под полным контролем, афганские граждане находятся в состоянии страха и смятения, как дипломаты, а представители международных организаций бегут из Афганистана.</t>
+  </si>
+  <si>
+    <t>Я видел людей в тюрбанах на головах с ружьями в руках, которые посреди ночи на своих «хондах» скандировали «Бог велик» и заходили в Спин-Болдак. Тогда я решил найти более безопасное место для моей семьи. Я уехал в Пакистан и пересек пограничные ворота Чамана. Жители Спин-Болдака знали, что они не могут продолжать безопасно жить в этом районе, опасаясь, что талибы придут с теми же намерениями, что и в прошлом.</t>
+  </si>
+  <si>
+    <t>Одна из групп, наиболее пострадавших от этой многолетней войны, - афганские женщины, которые теперь столкнулись с новой суровой реальностью. Они опасаются, что при талибах их ожидает потеря образа жизни, отсутствие доступа к образованию и полное нарушение основных прав.</t>
+  </si>
+  <si>
+    <t>В последние годы, хотя учебные программы по половому воспитанию оставались труднодостижимыми в большинстве арабских стран, несколько арабских женщин взяли на себя задачу предоставить альтернативу и предоставить информацию о сексе через социальные сети любопытным молодым мужчинам.</t>
+  </si>
+  <si>
+    <t>В остальном арабском мире половое воспитание остается в рамках консервативных границ уроков религии и биологии, поскольку оно ограничивается тщательно отобранными темами, такими как половое созревание, репродуктивная система и заболевания, передаваемые половым путем. Напротив, разговоры о сексуальности, фертильности, сексуальном насилии, безопасном сексе, понятиях согласия и разнообразия и т. Д. Ограничиваются шепотом учеников в школьных залах, часто основанном на ненаучном или порнографическом контенте в Интернете, если не полностью приглушенном.</t>
+  </si>
+  <si>
+    <t>Если мы продолжаем избегать этих разговоров и делать половое воспитание табу, мы на самом деле причиняем вред людям, которых пытаемся защитить. Мы подвергаем девочек жестокому обращению, слишком долго скрывая от них правду, делая их неподготовленными к своим отношениям и, возможно, более уязвимыми для жестокого обращения и нападений.</t>
+  </si>
+  <si>
+    <t>Они просят пожертвований после землетрясения, наводнения, пожара и пандемии. Конечно, мы сделаем все возможное, чтобы помочь нуждающимся, но сделают ли то же самое те, кто ведет нас и собирает с нас налоги?</t>
+  </si>
+  <si>
+    <t>«Многонациональное население Хузестана, в которое входит большая община арабов-иранцев, неоднократно жаловалось на нехватку чистой воды, но было встречено репрессивной политикой государства.
+С начала протестов митинги распространились на многие другие провинции, граждане выражают свою солидарность с жаждущими жителями Хузестана.</t>
+  </si>
+  <si>
+    <t>Новые протесты принадлежали низшему среднему классу, бедным, и в основном из районов и периферийных частей страны, в то время как зеленое движение, например, базировалось среди высшего среднего класса в больших городах. В то время как протестующие в последние два десятилетия в некоторой степени симпатизировали так называемой реформистской фракции, новая волна протестов не делает различий между различными фракциями режима и направлена ​​против всей Исламской Республики, режима, который не только репрессивен и жестокий, но также глубоко коррумпированный и некомпетентный.</t>
+  </si>
+  <si>
+    <t>Это дело было раскрыто теми же доказательствами, что и 10 лет назад, и если правосудие является одной из форм сдерживания людей от совершения преступлений, то безнаказанность в Колумбии является стимулом для совершения преступлений, если один из них не может быть осужден, даже если он виновен.</t>
+  </si>
+  <si>
+    <t>Государство должно публично осудить насилие в отношении журналистов, проводить расследования, привлекать к ответственности заслуживающих доверия виновных, возмездие за них и сдерживать тех, кто попрошайничает для совершения того же преступления в будущем</t>
+  </si>
+  <si>
+    <t>Колумбийское [правительство] приняло программу защиты журналистов под угрозой, которая до сих пор существует, но эта программа носит противоречивый характер, особенно после того, как журналисты утратили доверие к ней после установления сговора между силами безопасности, отвечающими за осуществление программы, и мишенью журналистов.</t>
+  </si>
+  <si>
+    <t>В сентябре Народная партия представила парламенту законопроект, в котором будет сформулирован принцип индивидуального банкротства, что изменит правила, касающиеся взыскания долгов.
+Хотя этот закон все еще находится на рассмотрении, его авторы утверждают, что при такой степени защиты отдельные лица не будут лишены своих домов.
+После перестрелки со смертельным исходом в Алматы, крупнейшем городе страны, должностные лица заявили, что «жестокая» практика взыскания долгов была главным мотивом для выстрела.
+Кроме того, я многому научился в области литературного перевода.</t>
+  </si>
+  <si>
+    <t>И я верю, что все еще учусь.
+Коммерческая сторона была очень труднодоступной с точки зрения авторских прав и т.д.
+Проект книги был начат в 2017 году. Книга наконец-то была опубликована в 2020 году.
+Так что, помимо ремесленных и коммерческих аспектов, я научился терпеливому и самодисциплине, чтобы выжить, несмотря на препятствия.</t>
+  </si>
+  <si>
+    <t>И наконец, я хочу быть и делать то, что хочу видеть в мире.
+Если я хочу, чтобы в Южной Азии было больше разных книг, которые можно было бы принять и прочитать, то я должен выполнить свой моральный долг.
+Я считаю, что позитивная энергия в этой работе более продуктивна, чем просто жаловаться на проблемы, которые я вижу на литературной арене.
+На данный момент, это индивидуальный риск, потому что я не могу заплатить кому-то, но я надеюсь, что смогу найти несколько вариантов финансирования, чтобы я мог заплатить некоторым персонажам за просмотры и интервью.
+Посмотрим.</t>
+  </si>
+  <si>
+    <t>История касается не здоровья заключенных, а здоровья самой страны.
+История о репрессивных инструментах, унаследованных от предыдущих поколений, взорвалась в соперничестве.
+Полное отторжение голоса и тела - самое сердце рассвета в битве.
+Мы считаем, что слово означает прямое решение продолжать вражду и причинять вред.
+Но если ты меня видишь и слышишь, шансы на то, что ты отступишь и успокоишься, остаются открытыми.
+И если мы не используем их, то по крайней мере, будем продолжать жить в авангарде.
+Величайшая вражда заключается в том, чтобы не видеть меня и не пытаться понять меня; чтобы я стал лишь материалом для изгнания, истребления, изоляции, изгнания или исключения, чтобы превратиться в символ или паранойю без физического физического существования.
+На рассвете ссора - это наследство, за которое платят все тела, и оно продолжает оплачиваться даже после окончания битвы.</t>
+  </si>
+  <si>
+    <t>Как защитить тела наших детей от наследия тюрьмы? Ответ не заканчивается, когда заключенные освобождаются, а начинается с освобождения и доходит до фантазий, которые стирают сами тюрьмы, а не заключенных.</t>
+  </si>
+  <si>
+    <t>Несмотря на то, что российская стратегия по водороду является самым свежим и самым подробным документом о видении Кремля в отношении водорода, она далека от того, чтобы существенно изменить правила игры в энергетическом секторе страны.
+На самом деле, как и многие другие аналогичные документы, которые, как предполагается, будут направлять развитие российской энергетической промышленности, они, похоже, являются реакцией, а не проактивностью, поскольку они были приняты более чем через год после того, как основные энергетические партнеры страны сформулировали свои стратегии в отношении водорода.</t>
+  </si>
+  <si>
+    <t>Некоторые называют водород швейцарским топливным ножом, который является уникальным во многих отношениях.
+Учитывая, что это самый богатый элемент во Вселенной, не будет недостатка в снабжении.
+Он может переключить энергию с (электрической) на (химическую) форму, хранить ее в течение долгого времени и перевозить туда, где это необходимо.
+Тем не менее, удивительно, что углекислый газ не вырабатывается при сжигании.
+На самом деле, только вода образуется как побочный продукт.</t>
+  </si>
+  <si>
+    <t>Многие сирийские молодые люди начали покидать южную часть Сирии с начала нынешнего 2021 года из-за нестабильности в регионе и из-за опасений, что они могут быть взяты на обязательную службу в армию сирийского режима и втянуты в боевые действия на севере страны.
+Многие из них согласились продать свои драгоценные вещи в Сирии, чтобы получить деньги, которые они платят торговцам в Ливии, чтобы доставить их в Италию и Мальту на лодках через Средиземное море.</t>
+  </si>
+  <si>
+    <t>Мы чуть не приблизились к итальянскому побережью, а потом приблизились к лодке, на которой мы ехали, и начали показывать нам свои руки, и мы решили сбежать, но судно спустилось на небольшую лодку с шестью вооруженными людьми, и они преследовали нас, а затем стреляли по двигателю нашей лодки, чтобы его отключить.</t>
+  </si>
+  <si>
+    <t>Европейский союз несет ответственность за варварство в Ливии, прямо или косвенно игнорируя ее действия. Вооруженные группы, выигрывающие от мигрантов, финансируются, а соучастие в этих преступлениях остается безнаказанным из-за невозможности требовать ответственности и ответственности за динамику переселения или передачи на внешний подряд контроля за иммиграцией.</t>
+  </si>
+  <si>
+    <t>Помимо выборов в Перу, состоявшихся в июне, в Интернете распространялась ложная информация о процессе выборов, многие из которых, как и другие страны, были связаны с попытками подорвать доверие к избирательным органам, а также с попытками обмануть использование ложной и правдивой информации в политических целях, как, например, распространение новостей о регистрации избирателей и указание на то, что в списках были имена умерших, но при этом отсутствовала информация о графике и процедуре изменения и закрытия списков.</t>
+  </si>
+  <si>
+    <t>В ходе этих протестов и демонстраций в Колумбии распространялась ложная информация, и местные источники сообщали, что сотни видеокассет, аудиозаписей и фотографий в Интернете были просмотрены в ходе общенациональной забастовки в Колумбии.</t>
+  </si>
+  <si>
+    <t>Кроме того, имели место акты насилия вне рамок массовых демонстраций; увеличилось число сообщений о словесных и фактических посягательствах на прессу со стороны высокопоставленных должностных лиц правительства, и с января 2021 года в Латинской Америке были убиты по меньшей мере четыре журналиста.</t>
+  </si>
+  <si>
+    <t>Теперь, после полного контроля движения &lt; &lt; Талибан &gt; &gt; , афганские граждане находятся в состоянии страха и волнений в качестве дипломатов, а представители международных организаций в настоящее время покидают Афганистан.</t>
+  </si>
+  <si>
+    <t>Я видел, как мужчины с тюрбанами на головах, с ружьями в руках, катались на мотоциклах Хонды посреди ночи, восклицая \"Бог Акбар\" и вступая в \"Большой мальчик\".
+Тогда я решил найти более безопасное место для своей семьи.
+Отбыла в Пакистан, пересекла пограничный контрольно-пропускной пункт в Шамане
+Жители Спин-Больдака знали, что они не могут жить в безопасности в этом районе, опасаясь, что талибы придут с теми же намерениями, которые они имели в прошлом.</t>
+  </si>
+  <si>
+    <t>Одна из групп, наиболее пострадавших от этой войны десятилетиями, это афганские женщины, которые сейчас сталкиваются с жестокой и новой реальностью.
+Они опасаются, что при режиме талибов их ждет утрата образа жизни и отсутствие доступа к образованию, а также полное нарушение основных прав.</t>
+  </si>
+  <si>
+    <t>В последние годы, несмотря на то, что в большинстве арабских стран учебные программы по половому воспитанию остаются недоступными, несколько арабских женщин взяли на себя задачу предоставления альтернативных вариантов и предоставления информации о сексе в социальных сетях молодежи, которая становится все более любопытной.</t>
+  </si>
+  <si>
+    <t>В остальной части арабского мира половое воспитание по-прежнему ограничивается рамками, установленными для изучения религии и биологии, и ограничивается тщательно отобранными дисциплинами, такими, как взрослая жизнь, репродуктивная система и заболевания, передаваемые половым путем.
+С другой стороны, разговоры о сексуальной активности, фертильности, сексуальном надругательстве, безопасном сексе или понятиях согласия и разнообразия между полами ограничиваются шепотами, которыми пользуются учащиеся в школьных коридорах, и часто основаны на ненаучном или порнографическом содержании в Интернете, если не полностью забытом.</t>
+  </si>
+  <si>
+    <t>Если мы будем продолжать избегать этих разговоров и считать половое воспитание запретом, мы на самом деле причиним вред тем, кого мы пытаемся защитить.
+Мы подвергаем девочек огромному насилию, скрывая от них правду долгое время, оставляя их неподготовленными к отношениям и, возможно, более уязвимыми к злоупотреблениям и злоупотреблениям.</t>
+  </si>
+  <si>
+    <t>Они просят о пожертвованиях после землетрясения, наводнения, пожаров и пандемий.
+Конечно, мы сделаем все, что в наших силах, чтобы помочь нуждающимся, но могут ли те, кто ведет нас, и мы должны платить налоги, делать то же самое?</t>
+  </si>
+  <si>
+    <t>Многоэтнические жители Хузестана, в том числе большая арабская иранская община, неоднократно жаловались на нехватку чистой воды, но они были скомпрометированы репрессивной политикой государства.
+С момента начала протестов во многих других мухафазах прошли марши, в ходе которых граждане выразили солидарность с жителями Хузестана.</t>
+  </si>
+  <si>
+    <t>Новые протесты относятся к низшему среднему классу и бедным слоям населения, главным образом к районам и периферийным районам страны, в то время как, например, зеленое движение было главным среди высшего среднего класса в крупных городах.
+В то время как в последние два десятилетия демонстранты в определенной степени симпатизировали так называемой реформистской фракции, новая волна протестов не проводит различия между различными фракциями режима и направлена против всего Исламского государства, которое является не только репрессивным и жестоким, но и крайне коррумпированным и неэффективным.</t>
+  </si>
+  <si>
+    <t>google_en-ru</t>
+  </si>
+  <si>
+    <t>api_en-ru</t>
+  </si>
+  <si>
+    <t>Это дело было разрешено с использованием тех же доказательств, что и у них, по крайней мере, 10 лет назад. Если правосудие - это форма отговора, призванная не допустить совершения преступлений людьми, то безнаказанность в Колумбии - это почти стимул, потому что действительно сложно осудить кого-либо, даже если он виновен.</t>
+  </si>
+  <si>
+    <t>Власти должны публично осуждать насилие в отношении журналистов, расследовать и привлекать их к ответственности заслуживающим доверия образом, чтобы наказать виновных и предотвратить подобные преступления в будущем.</t>
+  </si>
+  <si>
+    <t>Действительно, [правительство] Колумбии приняло программу защиты журналистов, находящихся под угрозой, которая действует и сегодня. Но история программы неоднозначна, особенно после того, как журналисты потеряли к ней доверие из-за убедительных доказательств сговора между силами безопасности, ведущими программу, и теми, кто нацелен на журналистов.</t>
+  </si>
+  <si>
+    <t>В сентябре Народная партия представила в парламент законопроект, который установит принцип индивидуального банкротства, который изменит правила привлечения к взысканию долгов. Хотя закон все еще находится на рассмотрении, его сторонники заявляют, что при такой защите люди не могут быть лишены жилища. После смертельного выстрела в Алматы, крупнейшем городе страны, депутаты мотивировали убийство «чудовищным» взысканием долгов.</t>
+  </si>
+  <si>
+    <t>Я также много узнал о художественном переводе. Думаю, я все еще учусь. Коммерческая сторона дела также была крутой кривой обучения с точки зрения получения разрешения на авторские права и т. Д. Я начал книжный проект в 2017 году, и книга, наконец, была выпущена в 2020 году. Так что, помимо ремесленных и коммерческих аспектов, я изучил искусство терпения и самодисциплины, чтобы не сбиться с курса, несмотря на неудачи.</t>
+  </si>
+  <si>
+    <t>Наконец, я хочу делать и быть в большей степени тем, что я хотел бы видеть в мире. Так что, если я хочу, чтобы книги из Южной Азии принимали и читали больше, мне нужно внести в это свою лепту литературного гражданства. Я считаю более продуктивным направлять положительную энергию через такую ​​работу, чем просто жаловаться на проблемы, которые я вижу в литературном ландшафте. Прямо сейчас это индивидуальное предприятие, потому что я не могу позволить себе никому платить, но я надеюсь найти некоторые варианты финансирования, чтобы я мог заплатить нескольким людям за интервью и обзоры. Посмотрим.</t>
+  </si>
+  <si>
+    <t>Речь идет не о здоровье заключенных, а о здоровье нации. Это история о жестоких орудиях, передаваемых из поколения в поколение, и о злобной вражде, которая будет унаследована будущими поколениями. Полное отрицание голоса и тела является толчком для вражды. Мы думаем о вражде как об умышленном решении продолжить вражду и причинить боль, но если вы видите и слышите меня, есть шанс для отступления и перемирия; даже если мы не воспользуемся этим, мы по крайней мере останемся в равных условиях. Когда бушует вражда, ты не видишь меня и не пытаешься понять. Я становлюсь объектом, чем-то, что должно быть устранено, разрушено, исчезло, отрицается, исключено; Я становлюсь символом или призраком без материального физического присутствия. Наследие вражды - это цена, которую платят все тела, и они продолжают платить ее даже после того, как вражда угасает.</t>
+  </si>
+  <si>
+    <t>Как нам защитить тела наших детей от тюремного наследия? Решение не ограничивается освобождением задержанных. Он начинается с освобождения, но должен заканчиваться творческим видением уничтожения тюрем, а не заключенных.</t>
+  </si>
+  <si>
+    <t>Хотя российская водородная стратегия является самым последним и подробным публично доступным документом о взглядах Кремля на водород, она далека от того, чтобы кардинально изменить правила игры в энергетическом секторе страны. Фактически, как и многие другие аналогичные документы, которые должны стимулировать развитие российской энергетики, он, похоже, носит скорее реактивный, чем упреждающий характер, поскольку он был принят более чем через год после того, как ключевые энергетические партнеры страны сформулировали свои собственные водородные стратегии.</t>
+  </si>
+  <si>
+    <t>Водород, который некоторые называют швейцарским армейским ножом топлива, уникален во многих отношениях. Поскольку он является самым распространенным элементом во Вселенной, его никогда не будет недостатка. Он может преобразовывать одну форму энергии (электрическую) в другую (химическую), хранить ее в течение длительного времени и транспортировать туда, где это необходимо. Однако наиболее примечательно то, что при сгорании он не выделяет углекислый газ. Фактически, он производит только воду в качестве побочного продукта.</t>
+  </si>
+  <si>
+    <t>Многие молодые сирийцы покинули юг Сирии с начала 2021 года из-за нестабильности в регионе и их страха быть втянутыми в обязательную военную службу и брошенными на передовую на севере страны. Многие из них продавали свои ценности в Сирии, чтобы получить деньги, необходимые для оплаты контрабандистам в Ливии, чтобы они доставили их в Италию и на Мальту на лодке через Средиземное море. Но многие так и не завершили путешествие.</t>
+  </si>
+  <si>
+    <t>Мы собирались достичь итальянского побережья, когда к лодке, на которую мы садились, подошел корабль. Они начали указывать на нас. Мы решили бежать, но корабль спустил небольшую лодку с шестью вооруженными людьми, которые погнались за нашей лодкой, а затем выстрелили в ее двигатель, остановив его. Тогда к нам подошел корабль, и нас перевели на него, где было еще около 600 иммигрантов разных национальностей.</t>
+  </si>
+  <si>
+    <t>Европейский Союз несет ответственность за варварство Ливии напрямую или закрывая глаза на ее действия, поскольку вооруженные группы, получающие прибыль от мигрантов, финансируются, а соучастие в этих преступлениях остается безнаказанным из-за невозможности требовать ответственности и ответственности в динамике переселения. или аутсорсинг миграционного контроля.</t>
+  </si>
+  <si>
+    <t>На июньских выборах в Перу как в Интернете, так и в автономном режиме распространялась дезинформация в отношении избирательных процедур; большая часть его, как видно из других стран, пытается подорвать доверие к избирательным органам. Помимо ложной информации, реальная информация использовалась в политических целях. Например, распространялись новости о списках избирателей, внесенных в реестр, что указывало на то, что в них были включены имена умерших лиц, но не содержалась информация о сроках и процедурах исправления и доработки списков.</t>
+  </si>
+  <si>
+    <t>Дезинформация была в изобилии и во время этих протестов, например, во время демонстраций в Колумбии. Местные источники сообщают, что в Интернете распространяются сотни видео, аудиозаписей и изображений о национальной забастовке Колумбии, многие из которых содержат ложь или информацию, вырванную из контекста, что существенно влияет на повествование о том, что на самом деле происходило на улицах.</t>
+  </si>
+  <si>
+    <t>Насилие также имеет место вне контекста публичных демонстраций. Стигматизирующие выступления и словесные нападки на прессу все чаще исходят от высокопоставленных государственных чиновников. С января 2021 года в Латинской Америке были убиты как минимум четыре журналиста.</t>
+  </si>
+  <si>
+    <t>Теперь, когда Талибан получил полный контроль, афганские граждане остались в страхе и неуверенности как дипломаты, а представители международных организаций бегут из Афганистана.</t>
+  </si>
+  <si>
+    <t>Я видел мужчин в тюрбанах на головах и с винтовками в руках на мотоциклах Honda посреди ночи, скандировавших «Аллах-у-Акбар» и входивших в Спин Болдак. Именно тогда я решил найти более безопасное место для своей семьи. Я уехал в Пакистан, пересек пограничные ворота Чаман. Жители Спин-Болдака знали, что они не могут продолжать безопасно жить в этом районе, опасаясь, что талибы пришли с теми же намерениями, что и в прошлом.</t>
+  </si>
+  <si>
+    <t>Одна из групп, наиболее пострадавших от продолжавшейся десятилетия войны, - это афганские женщины, которые теперь столкнулись с суровой и новой реальностью. Они опасаются, что потеря их образа жизни и доступа к образованию наряду с полным нарушением основных прав - вот что их ждет при талибах.</t>
+  </si>
+  <si>
+    <t>В последние годы, поскольку учебные программы по половому воспитанию остаются недоступными в большинстве арабских стран, несколько арабских женщин взяли на себя задачу предоставить альтернативы, предлагая информацию о сексе через социальные сети все более любознательной молодежи.</t>
+  </si>
+  <si>
+    <t>В остальном арабском мире половое воспитание ограничено консервативными рамками уроков религии и биологии, ограничено тщательно подобранными темами, такими как половое созревание, репродуктивная система и заболевания, передаваемые половым путем. Между тем, разговоры о сексуальности, фертильности, сексуальном насилии и безопасном сексе или о таких концепциях, как согласие и гендерное разнообразие, сводятся к шепоту среди учеников в школьных коридорах, часто основанным на ненаучном или порнографическом онлайн-контенте, если не полностью приглушенном.</t>
+  </si>
+  <si>
+    <t>Если мы продолжаем избегать этих разговоров и относиться к половому воспитанию как к табу, мы, по сути, причиняем вред только тем, кого пытаемся защитить. Мы оказываем девочкам огромную медвежью услугу, слишком долго держим их в неведении, это делает их неподготовленными к своим отношениям и даже может сделать их более уязвимыми для жестокого обращения.</t>
+  </si>
+  <si>
+    <t>Просят пожертвования после землетрясения, наводнения, пожара, во время пандемии. Конечно, мы сделаем все, что в наших силах, чтобы помочь нуждающимся, но сделают ли те, кто собирает наши налоги и руководит нами, то же самое?</t>
+  </si>
+  <si>
+    <t>Многонациональное население Хузестана, которое включает в себя большую общину этнических арабов-иранцев, неоднократно жаловалось на нехватку чистой воды только для того, чтобы встречаться с репрессивной политикой государства._x000D_
+С тех пор, как начались протесты, митинги прокатились по нескольким другим провинциям, и граждане выразили солидарность с жаждущим народом Хузестана .</t>
+  </si>
+  <si>
+    <t>Новые протесты принадлежат низшему среднему классу и бедным и происходят в основном из районов и периферийных частей страны, в то время как движение зеленых, например, базируется на верхнем среднем классе в крупных городах. В то время как протестующие в последние два десятилетия до некоторой степени симпатизировали так называемой реформистской фракции, новая волна протестов не проводит различий между различными фракциями режима и направлена ​​против всего Государства Исламская Республика - истеблишмента, который является не только репрессивным и жестоким, но также чрезвычайно коррумпированным и некомпетентным.</t>
+  </si>
+  <si>
+    <t>Это дело было урегулировано с использованием тех же доказательств, что и по меньшей мере 10 лет назад.
+Если правосудие является одной из форм устрашения, чтобы не допустить совершения людьми преступлений, то безнаказанность в Колумбии является практически стимулом, поскольку действительно трудно, чтобы кто-то был осужден, даже несмотря на то, что он виновен.</t>
+  </si>
+  <si>
+    <t>Действительно, [правительство] Колумбии приняло программу защиты журналистов, находящихся под угрозой, которая до сих пор действует.
+Но эта программа имеет смешанный послужной список, особенно после того, как журналисты потеряли доверие к ней из-за убедительных доказательств сговора между силами безопасности, осуществляющими эту программу, и теми, кто нацелился на журналистов.</t>
+  </si>
+  <si>
+    <t>В сентябре Народная партия представила на рассмотрение парламента законопроект, устанавливающий принцип индивидуального банкротства, который изменит правила ведения боевых действий в целях взыскания задолженности.
+Хотя этот закон все еще находится на рассмотрении, его сторонники утверждают, что при такой защите люди не могут быть лишены своего дома.
+После смертельной стрельбы в Алма-Ате, крупнейшем городе страны, депутаты назвали в качестве мотива стрелявшего чудовищную практику сбора долгов.</t>
+  </si>
+  <si>
+    <t>Кроме того, я многому научился по ходу работы над литературным переводом.
+Я все еще учусь, полагаю.
+Коммерческая сторона вещей также была крутой кривой обучения с точки зрения получения авторского права и т.д. Я начал книжный проект в 2017 году, а книга, наконец, была запущена в 2020 году.
+Так что, помимо ремесленных и коммерческих аспектов, я научился искусству терпения и самодисциплины, чтобы оставаться в курсе дела, несмотря на неудачи.</t>
+  </si>
+  <si>
+    <t>Наконец-то, я хочу сделать и быть больше из того, что я хотел бы видеть в мире.
+Так что, если я хочу видеть, как принимают и читают более разнообразные книги из Южной Азии, мне нужно сделать свою часть литературного гражданства для этого.
+Я считаю более продуктивным использовать позитивную энергию в этой работе, чем просто жаловаться на проблемы, которые я вижу по всему литературному ландшафту.
+Сейчас это сольное предприятие, потому что я не могу позволить себе платить кому-либо, но я надеюсь найти варианты финансирования, чтобы я мог заплатить паре людей за интервью и отзывы.
+Посмотрим.</t>
+  </si>
+  <si>
+    <t>Речь идет не о здоровье заключенных, а о здоровье нации.
+Это история о репрессивных инструментах, переданных поколениям, и о жестокой вражде, которая будет унаследована будущими поколениями.
+Полное отрицание голоса и тела является импульсом вражды.
+Мы считаем вражду преднамеренным решением продолжать вражду и причинять боль, но если вы увидите и услышите меня, есть шанс на отступление и перемирие; даже если мы не воспользуемся ею, мы, по крайней мере, остаемся на равных.
+Когда вражда бушует, ты не видишь и не пытаешься понять меня.
+Я становлюсь объектом, что-то, что нужно уничтожить, уничтожить, исчезнуть, отменить, исключить; я становлюсь символом или богейманом, без материального, физического присутствия.
+Враждебное наследие - это цена, которую платят все тела, и они продолжают платить за это даже после того, как вражда исчезнет.</t>
+  </si>
+  <si>
+    <t>Как защитить тела наших детей от этого наследия тюрем?
+Решение этой проблемы не ограничивается освобождением задержанных.
+Она начинается с освобождения, но должна закончиться творческим видением стирания тюрем, а не заключенных.</t>
+  </si>
+  <si>
+    <t>Хотя российская водородная стратегия является самым последним и подробным общедоступным документом о Кремлях, размышляющих о водороде, она далека от радикального изменения правил игры в энергетическом секторе страны.
+На самом деле, как и многие другие аналогичные документы, которые призваны стимулировать развитие российской энергетической промышленности, она, как представляется, носит скорее реактивный, чем проактивный характер, поскольку она была принята более чем через год после того, как ключевые энергетические партнеры стран разработали свои собственные стратегии в области водорода.</t>
+  </si>
+  <si>
+    <t>Поврежденный некоторыми швейцарскими армейскими ножами топлива, водород уникален во многих отношениях.
+Поскольку вселенная является самым богатым элементом, она никогда не будет в дефиците.
+Она может преобразовывать одну форму энергии (электрической) в другую (химическую), хранить ее в течение длительного времени и перевозиться туда, где она необходима. Однако самое удивительное заключается в том, что он не излучает углекислый газ при возгорании.
+На самом деле, она производит только воду в качестве побочного продукта.</t>
+  </si>
+  <si>
+    <t>Многие молодые сирийцы покинули южную часть Сирии с начала 2021 года из-за нестабильности в регионах и из-за боязни быть втянутыми в обязательную военную службу и брошенными на фронты северных стран. Многие из них продали свои ценности в Сирии, чтобы получить деньги, необходимые контрабандистам в Ливии, чтобы доставить их в Италию и Мальту на лодке через Средиземное море. Но многие так и не завершили это путешествие.</t>
+  </si>
+  <si>
+    <t>Мы собирались доплыть до итальянского побережья, когда корабль приблизился к лодке, которую мы высадили.
+Они начали указывать на нас.
+Мы решили сбежать, но корабль опустился на маленькую лодку с шестью вооруженными людьми, которые погнались за нашей лодкой, а затем застрелили ее двигатель, в результате чего она остановилась.
+Корабль подошел к нам тогда, и они перевели нас туда, где было около 600 других иммигрантов различных национальностей.</t>
+  </si>
+  <si>
+    <t>Европейский союз несет ответственность за варварство в Ливии либо непосредственно, либо закрывая глаза на ее действия, поскольку финансовые средства выделяются вооруженным группам, которые получают доходы от мигрантов, и соучастие в этих преступлениях остается безнаказанным из-за невозможности взять на себя ответственность и ответственность за динамику переселения или аутсорсировать миграционный контроль.</t>
+  </si>
+  <si>
+    <t>В ходе выборов в Перу, состоявшихся в июне, дезинформация распространялась как в режиме онлайн, так и в режиме офлайн в связи с избирательными процедурами; многие из них, как видно из других стран, пытались подорвать доверие к избирательным органам.
+Помимо ложной информации, реальная информация манипулируется в политических целях.
+Например, распространялись сообщения о списках избирателей, в которых указывалось, что они включали имена умерших лиц, но при этом отсутствовала информация о сроках и процедуре составления и окончательной доработки списков.</t>
+  </si>
+  <si>
+    <t>В ходе этих протестов, как, например, во время демонстраций в Колумбии, также было много дезинформации.
+Местные источники сообщили, что сотни видео, аудиозаписей и изображений распространяются в Интернете о национальной забастовке Колумбии, многие из которых содержат ложь или информацию, заимствованную из контекста, что оказывает значительное влияние на повествование о том, что на самом деле происходит на улицах.</t>
+  </si>
+  <si>
+    <t>Насилие также имеет место вне контекста публичных демонстраций.
+Стигматизирующие высказывания и словесные нападки на прессу все чаще происходят от высокопоставленных государственных должностных лиц.
+С января 2021 года в Латинской Америке было убито по меньшей мере четыре журналиста.</t>
+  </si>
+  <si>
+    <t>Я видел людей с тюрбанами на головах и винтовками в руках, на мотоциклах Хонды посреди ночи, которые скандировали Аллах-у-Акбар и вошли в Спин-Болдак.
+Тогда я решил найти более безопасное место для своей семьи.
+Я уехала в Пакистан, пересекая границы с Чаманом.
+Жители Спин-Болдака знали, что они не могут продолжать безопасно жить в этом районе, опасаясь, что талибы пришли с теми же намерениями, что и в прошлом.</t>
+  </si>
+  <si>
+    <t>Одной из групп, в наибольшей степени пострадавших от продолжавшейся десятилетия войны, являются афганские женщины, которые в настоящее время сталкиваются с жестокой и новой реальностью.
+Они опасаются, что утрата их образа жизни и их доступ к образованию наряду с полным нарушением основных прав -- вот то, что ожидает их в рамках движения &amp;lt; &amp;lt; Талибан &amp;gt; &amp;gt; .</t>
+  </si>
+  <si>
+    <t>В остальной части арабского мира половое воспитание ограничивается консервативными границами религиозных и биологических классов, а также тщательно отобранными предметами, такими, как половое созревание, репродуктивная система и болезни, передаваемые половым путем.
+Между тем разговоры о сексуальности, фертильности, сексуальных надругательствах и безопасном сексе, или такие понятия, как согласие и гендерное разнообразие, сводятся к шепотам среди учащихся в школьных коридорах, часто основанных на ненаучных или порнографических онлайн-контентах, если не полностью заглушены.</t>
+  </si>
+  <si>
+    <t>Если мы и впредь будем избегать этих разговоров и относиться к половому воспитанию как к табу, то на самом деле мы причиняем вред только тем, кого пытаемся защитить.
+Мы оказываем девочкам огромную плохую услугу, удерживая их в неведении слишком долго, это оставляет их не готовыми к своим отношениям и может даже сделать их более уязвимыми к злоупотреблениям.</t>
+  </si>
+  <si>
+    <t>Они просят о пожертвованиях после землетрясения, наводнения, пожара во время пандемии.
+Конечно, мы будем делать то, что в наших силах, чтобы помочь нуждающимся, но будут ли и те, кто собирает наши налоги и руководит нами, делать то же самое?</t>
+  </si>
+  <si>
+    <t>Многоэтничное население Хузестана, в состав которого входит большая община этнических арабских иранцев, неоднократно жалуется на отсутствие чистой воды, лишь для того, чтобы противостоять репрессивной политике со стороны штатов.
+С тех пор, как начались протесты, митинги охватили несколько других провинций, и граждане выразили солидарность с жаждущим народом Хузестана.</t>
+  </si>
+  <si>
+    <t>Новые протесты относятся к низшему среднему классу и бедным слоям населения и происходят главным образом из районов и периферийных районов страны, в то время как движение &amp;lt; &amp;lt; Зеленый &amp;gt; &amp;gt; , например, имеет свою основу среди высшего среднего класса в крупных городах.
+В то время как протестующие за последние два десятилетия в определенной степени симпатизировали так называемой реформистской фракции, новая волна протестов не проводит различий между различными фракциями режима и выступает против всего государственного образования Исламской Республики, которое не только является репрессивным и жестоким, но и чрезвычайно коррумпированным и некомпетентным.</t>
   </si>
 </sst>
 </file>
@@ -1200,20 +1577,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="44.7109375" defaultRowHeight="198" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="3" customWidth="1"/>
-    <col min="2" max="8" width="44.7109375" style="4"/>
-    <col min="9" max="16384" width="44.7109375" style="2"/>
+    <col min="1" max="1" width="4.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="37.28515625" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="44.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="16" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -1224,22 +1601,34 @@
         <v>80</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1250,22 +1639,34 @@
         <v>108</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1276,22 +1677,34 @@
         <v>109</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1302,22 +1715,34 @@
         <v>110</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G4" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1328,22 +1753,34 @@
         <v>111</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="G5" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1354,22 +1791,34 @@
         <v>112</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="G6" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="L6" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1380,22 +1829,34 @@
         <v>113</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="G7" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="J7" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="375" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1406,22 +1867,34 @@
         <v>114</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="G8" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="L8" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1432,22 +1905,34 @@
         <v>115</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="G9" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="L9" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1458,22 +1943,34 @@
         <v>116</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="G10" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="L10" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1484,22 +1981,34 @@
         <v>117</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="G11" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="L11" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1510,22 +2019,34 @@
         <v>118</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="G12" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="K12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="L12" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1536,22 +2057,34 @@
         <v>119</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="K13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="L13" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1562,22 +2095,34 @@
         <v>120</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="G14" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="J14" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="L14" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1588,22 +2133,34 @@
         <v>121</v>
       </c>
       <c r="D15" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="G15" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="J15" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="K15" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="L15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1614,22 +2171,34 @@
         <v>122</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="G16" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="J16" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="K16" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="L16" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1640,22 +2209,34 @@
         <v>123</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="G17" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="K17" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="L17" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1666,22 +2247,34 @@
         <v>124</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="G18" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="J18" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="K18" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="L18" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1692,22 +2285,34 @@
         <v>125</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="G19" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="K19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1718,22 +2323,34 @@
         <v>126</v>
       </c>
       <c r="D20" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="G20" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="J20" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="L20" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1744,22 +2361,34 @@
         <v>127</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="G21" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="K21" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="L21" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1770,22 +2399,34 @@
         <v>128</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="G22" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="J22" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="L22" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1796,22 +2437,34 @@
         <v>129</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="G23" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="J23" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="K23" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="L23" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1822,22 +2475,34 @@
         <v>130</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="G24" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="J24" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="K24" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="L24" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1848,22 +2513,34 @@
         <v>131</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="G25" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="K25" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="L25" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -1874,18 +2551,30 @@
         <v>132</v>
       </c>
       <c r="D26" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="G26" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="I26" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="J26" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="K26" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="L26" s="9" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
train experience and edited requirements
</commit_message>
<xml_diff>
--- a/reports/test_dataset_result.xlsx
+++ b/reports/test_dataset_result.xlsx
@@ -9,11 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="all" sheetId="1" r:id="rId1"/>
+    <sheet name="en_ru" sheetId="3" r:id="rId2"/>
+    <sheet name="ar_ru" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">all!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">ar_ru!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">en_ru!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="284">
   <si>
     <t>Русский</t>
   </si>
@@ -1108,7 +1115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1126,6 +1133,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1135,7 +1150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1243,11 +1258,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1296,6 +1384,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1577,10 +1701,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.7109375" defaultRowHeight="198" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1590,7 +1718,7 @@
     <col min="13" max="16384" width="44.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="16" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -2579,7 +2707,1097 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="34" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="48.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" style="19" customWidth="1"/>
+    <col min="2" max="6" width="61.7109375" style="20" customWidth="1"/>
+    <col min="7" max="16384" width="48.7109375" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="27" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="187.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="23">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="187.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="262.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="300" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>7</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>8</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="281.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>9</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="243.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="206.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>11</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>12</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="187.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <v>13</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="262.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>14</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="206.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>17</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <v>18</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>19</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="281.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
+        <v>21</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <v>22</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="21">
+        <v>23</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="187.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <v>24</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="318.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>25</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="44.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="61.7109375" style="20" customWidth="1"/>
+    <col min="7" max="16384" width="44.7109375" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="17" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="23">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="300" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="206.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="318.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>7</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>8</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="281.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>9</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="243.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>11</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="206.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>12</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <v>13</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="262.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>14</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>17</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <v>18</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>19</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="300" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
+        <v>21</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="187.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <v>22</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="21">
+        <v>23</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <v>24</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="300" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>25</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="46" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>